<commit_message>
update the example - quick fix but will need to do something programatically
</commit_message>
<xml_diff>
--- a/excel_templates/apartment-template.xlsx
+++ b/excel_templates/apartment-template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Number of bedrooms</t>
   </si>
@@ -41,12 +41,18 @@
   <si>
     <t>Name</t>
   </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>May Thi Nghe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +187,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +372,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -538,7 +562,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -549,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -870,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +914,7 @@
     <col min="1" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -904,25 +937,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>501</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6">
+        <v>132</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -931,7 +981,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -940,7 +990,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -949,7 +999,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -958,7 +1008,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -967,7 +1017,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -976,7 +1026,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -985,7 +1035,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -994,7 +1044,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1003,7 +1053,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1012,7 +1062,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1021,7 +1071,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1030,7 +1080,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>